<commit_message>
Added Program Academics Hex View and Related View
</commit_message>
<xml_diff>
--- a/Project Statistics/LOC.xlsx
+++ b/Project Statistics/LOC.xlsx
@@ -538,6 +538,9 @@
                 <c:pt idx="55">
                   <c:v>6198.0</c:v>
                 </c:pt>
+                <c:pt idx="57">
+                  <c:v>6361.0</c:v>
+                </c:pt>
                 <c:pt idx="60">
                   <c:v>6700.0</c:v>
                 </c:pt>
@@ -557,11 +560,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2119837816"/>
-        <c:axId val="-2127410664"/>
+        <c:axId val="2099800920"/>
+        <c:axId val="2099803928"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="-2119837816"/>
+        <c:axId val="2099800920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -571,14 +574,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2127410664"/>
+        <c:crossAx val="2099803928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-2127410664"/>
+        <c:axId val="2099803928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -589,7 +592,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2119837816"/>
+        <c:crossAx val="2099800920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -970,8 +973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="L58" sqref="L58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1323,6 +1326,9 @@
       <c r="A59" s="1">
         <v>41789</v>
       </c>
+      <c r="B59">
+        <v>6361</v>
+      </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="1">

</xml_diff>

<commit_message>
Implemented Program Courses View
</commit_message>
<xml_diff>
--- a/Project Statistics/LOC.xlsx
+++ b/Project Statistics/LOC.xlsx
@@ -541,11 +541,11 @@
                 <c:pt idx="57">
                   <c:v>6361.0</c:v>
                 </c:pt>
-                <c:pt idx="60">
-                  <c:v>6700.0</c:v>
+                <c:pt idx="58">
+                  <c:v>6765.0</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>10000.0</c:v>
+                  <c:v>9000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -560,11 +560,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2099800920"/>
-        <c:axId val="2099803928"/>
+        <c:axId val="680407944"/>
+        <c:axId val="541431944"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="2099800920"/>
+        <c:axId val="680407944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -574,14 +574,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099803928"/>
+        <c:crossAx val="541431944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2099803928"/>
+        <c:axId val="541431944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -592,7 +592,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099800920"/>
+        <c:crossAx val="680407944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -973,8 +973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I50" sqref="I50"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1334,6 +1334,9 @@
       <c r="A60" s="1">
         <v>41790</v>
       </c>
+      <c r="B60">
+        <v>6765</v>
+      </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="1">
@@ -1350,9 +1353,6 @@
       <c r="A62" s="1">
         <v>41792</v>
       </c>
-      <c r="B62">
-        <v>6700</v>
-      </c>
       <c r="C62" t="s">
         <v>9</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>41821</v>
       </c>
       <c r="B91">
-        <v>10000</v>
+        <v>9000</v>
       </c>
     </row>
     <row r="92" spans="1:2">

</xml_diff>

<commit_message>
Added Settings View Controller Authors
</commit_message>
<xml_diff>
--- a/Project Statistics/LOC.xlsx
+++ b/Project Statistics/LOC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27640" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -547,6 +547,9 @@
                 <c:pt idx="59">
                   <c:v>7119.0</c:v>
                 </c:pt>
+                <c:pt idx="79">
+                  <c:v>7116.0</c:v>
+                </c:pt>
                 <c:pt idx="89">
                   <c:v>10000.0</c:v>
                 </c:pt>
@@ -563,11 +566,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2078616760"/>
-        <c:axId val="2078619592"/>
+        <c:axId val="2055427704"/>
+        <c:axId val="2099595656"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="2078616760"/>
+        <c:axId val="2055427704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -577,14 +580,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2078619592"/>
+        <c:crossAx val="2099595656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2078619592"/>
+        <c:axId val="2099595656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -595,7 +598,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2078616760"/>
+        <c:crossAx val="2055427704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -976,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1460,6 +1463,9 @@
       <c r="A81" s="1">
         <v>41811</v>
       </c>
+      <c r="B81">
+        <v>7116</v>
+      </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="1">

</xml_diff>

<commit_message>
Implemented Main Favorites Tab
</commit_message>
<xml_diff>
--- a/Project Statistics/LOC.xlsx
+++ b/Project Statistics/LOC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21160" tabRatio="500"/>
+    <workbookView xWindow="-24260" yWindow="5000" windowWidth="24260" windowHeight="15560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -103,8 +103,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -116,13 +122,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -532,12 +544,21 @@
                 <c:pt idx="51">
                   <c:v>5741.0</c:v>
                 </c:pt>
+                <c:pt idx="52">
+                  <c:v>5741.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>5741.0</c:v>
+                </c:pt>
                 <c:pt idx="54">
                   <c:v>6170.0</c:v>
                 </c:pt>
                 <c:pt idx="55">
                   <c:v>6198.0</c:v>
                 </c:pt>
+                <c:pt idx="56">
+                  <c:v>6198.0</c:v>
+                </c:pt>
                 <c:pt idx="57">
                   <c:v>6361.0</c:v>
                 </c:pt>
@@ -547,8 +568,68 @@
                 <c:pt idx="59">
                   <c:v>7119.0</c:v>
                 </c:pt>
+                <c:pt idx="60">
+                  <c:v>7119.0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>7119.0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>7119.0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>7119.0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>7119.0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>7119.0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>7119.0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>7119.0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>7119.0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>7119.0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>7119.0</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>7119.0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>7119.0</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>7119.0</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>7119.0</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>7119.0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>7119.0</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>7119.0</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>7119.0</c:v>
+                </c:pt>
                 <c:pt idx="79">
                   <c:v>7116.0</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>8305.0</c:v>
                 </c:pt>
                 <c:pt idx="89">
                   <c:v>10000.0</c:v>
@@ -566,11 +647,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2055427704"/>
-        <c:axId val="2099595656"/>
+        <c:axId val="2095332728"/>
+        <c:axId val="2095335656"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="2055427704"/>
+        <c:axId val="2095332728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -580,14 +661,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099595656"/>
+        <c:crossAx val="2095335656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2099595656"/>
+        <c:axId val="2095335656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -598,7 +679,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2055427704"/>
+        <c:crossAx val="2095332728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -980,7 +1061,7 @@
   <dimension ref="A1:D109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1298,11 +1379,17 @@
       <c r="A54" s="1">
         <v>41784</v>
       </c>
+      <c r="B54">
+        <v>5741</v>
+      </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="1">
         <v>41785</v>
       </c>
+      <c r="B55">
+        <v>5741</v>
+      </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="1">
@@ -1327,6 +1414,9 @@
       <c r="A58" s="1">
         <v>41788</v>
       </c>
+      <c r="B58">
+        <v>6198</v>
+      </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="1">
@@ -1362,6 +1452,9 @@
       <c r="A62" s="1">
         <v>41792</v>
       </c>
+      <c r="B62">
+        <v>7119</v>
+      </c>
       <c r="C62" t="s">
         <v>9</v>
       </c>
@@ -1373,90 +1466,144 @@
       <c r="A63" s="1">
         <v>41793</v>
       </c>
+      <c r="B63">
+        <v>7119</v>
+      </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="1">
         <v>41794</v>
       </c>
-    </row>
-    <row r="65" spans="1:1">
+      <c r="B64">
+        <v>7119</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
       <c r="A65" s="1">
         <v>41795</v>
       </c>
-    </row>
-    <row r="66" spans="1:1">
+      <c r="B65">
+        <v>7119</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
       <c r="A66" s="1">
         <v>41796</v>
       </c>
-    </row>
-    <row r="67" spans="1:1">
+      <c r="B66">
+        <v>7119</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
       <c r="A67" s="1">
         <v>41797</v>
       </c>
-    </row>
-    <row r="68" spans="1:1">
+      <c r="B67">
+        <v>7119</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
       <c r="A68" s="1">
         <v>41798</v>
       </c>
-    </row>
-    <row r="69" spans="1:1">
+      <c r="B68">
+        <v>7119</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
       <c r="A69" s="1">
         <v>41799</v>
       </c>
-    </row>
-    <row r="70" spans="1:1">
+      <c r="B69">
+        <v>7119</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
       <c r="A70" s="1">
         <v>41800</v>
       </c>
-    </row>
-    <row r="71" spans="1:1">
+      <c r="B70">
+        <v>7119</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
       <c r="A71" s="1">
         <v>41801</v>
       </c>
-    </row>
-    <row r="72" spans="1:1">
+      <c r="B71">
+        <v>7119</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
       <c r="A72" s="1">
         <v>41802</v>
       </c>
-    </row>
-    <row r="73" spans="1:1">
+      <c r="B72">
+        <v>7119</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
       <c r="A73" s="1">
         <v>41803</v>
       </c>
-    </row>
-    <row r="74" spans="1:1">
+      <c r="B73">
+        <v>7119</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
       <c r="A74" s="1">
         <v>41804</v>
       </c>
-    </row>
-    <row r="75" spans="1:1">
+      <c r="B74">
+        <v>7119</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
       <c r="A75" s="1">
         <v>41805</v>
       </c>
-    </row>
-    <row r="76" spans="1:1">
+      <c r="B75">
+        <v>7119</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
       <c r="A76" s="1">
         <v>41806</v>
       </c>
-    </row>
-    <row r="77" spans="1:1">
+      <c r="B76">
+        <v>7119</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
       <c r="A77" s="1">
         <v>41807</v>
       </c>
-    </row>
-    <row r="78" spans="1:1">
+      <c r="B77">
+        <v>7119</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
       <c r="A78" s="1">
         <v>41808</v>
       </c>
-    </row>
-    <row r="79" spans="1:1">
+      <c r="B78">
+        <v>7119</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
       <c r="A79" s="1">
         <v>41809</v>
       </c>
-    </row>
-    <row r="80" spans="1:1">
+      <c r="B79">
+        <v>7119</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
       <c r="A80" s="1">
         <v>41810</v>
+      </c>
+      <c r="B80">
+        <v>7119</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1495,6 +1642,9 @@
     <row r="87" spans="1:2">
       <c r="A87" s="1">
         <v>41817</v>
+      </c>
+      <c r="B87">
+        <v>8305</v>
       </c>
     </row>
     <row r="88" spans="1:2">

</xml_diff>

<commit_message>
Implemented School Detail View Controller
</commit_message>
<xml_diff>
--- a/Project Statistics/LOC.xlsx
+++ b/Project Statistics/LOC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-24260" yWindow="5000" windowWidth="24260" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24180" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -632,7 +632,7 @@
                   <c:v>8305.0</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>10000.0</c:v>
+                  <c:v>8703.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -647,11 +647,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2095332728"/>
-        <c:axId val="2095335656"/>
+        <c:axId val="2081972008"/>
+        <c:axId val="2081974872"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="2095332728"/>
+        <c:axId val="2081972008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -661,14 +661,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2095335656"/>
+        <c:crossAx val="2081974872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2095335656"/>
+        <c:axId val="2081974872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -679,7 +679,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2095332728"/>
+        <c:crossAx val="2081972008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1060,8 +1060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B87" sqref="B87"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1667,7 +1667,7 @@
         <v>41821</v>
       </c>
       <c r="B91">
-        <v>10000</v>
+        <v>8703</v>
       </c>
     </row>
     <row r="92" spans="1:2">

</xml_diff>

<commit_message>
User Interface Overhaul and Big fixes, Up updated Current Screenshots
</commit_message>
<xml_diff>
--- a/Project Statistics/LOC.xlsx
+++ b/Project Statistics/LOC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24180" windowHeight="15620" tabRatio="500"/>
+    <workbookView xWindow="-24260" yWindow="5600" windowWidth="24260" windowHeight="15560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -634,6 +634,9 @@
                 <c:pt idx="89">
                   <c:v>8703.0</c:v>
                 </c:pt>
+                <c:pt idx="92">
+                  <c:v>9483.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -647,11 +650,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2081972008"/>
-        <c:axId val="2081974872"/>
+        <c:axId val="2115439800"/>
+        <c:axId val="2115442744"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="2081972008"/>
+        <c:axId val="2115439800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -661,14 +664,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2081974872"/>
+        <c:crossAx val="2115442744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2081974872"/>
+        <c:axId val="2115442744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -679,7 +682,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2081972008"/>
+        <c:crossAx val="2115439800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1060,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1684,6 +1687,9 @@
       <c r="A94" s="1">
         <v>41824</v>
       </c>
+      <c r="B94">
+        <v>9483</v>
+      </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="1">

</xml_diff>

<commit_message>
Added Calendar Application Progress Button saving function under program academics view plus Bug fixes. Reached 40,000 lines milestone
</commit_message>
<xml_diff>
--- a/Project Statistics/LOC.xlsx
+++ b/Project Statistics/LOC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-24260" yWindow="5600" windowWidth="24260" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="-24180" yWindow="5600" windowWidth="24180" windowHeight="15560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -637,6 +637,12 @@
                 <c:pt idx="92">
                   <c:v>9483.0</c:v>
                 </c:pt>
+                <c:pt idx="93">
+                  <c:v>9691.0</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>9925.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -650,11 +656,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2115439800"/>
-        <c:axId val="2115442744"/>
+        <c:axId val="2077291224"/>
+        <c:axId val="2077294168"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="2115439800"/>
+        <c:axId val="2077291224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -664,14 +670,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115442744"/>
+        <c:crossAx val="2077294168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2115442744"/>
+        <c:axId val="2077294168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -682,7 +688,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115439800"/>
+        <c:crossAx val="2077291224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1063,8 +1069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1695,10 +1701,16 @@
       <c r="A95" s="1">
         <v>41825</v>
       </c>
+      <c r="B95">
+        <v>9691</v>
+      </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" s="1">
         <v>41826</v>
+      </c>
+      <c r="B96">
+        <v>9925</v>
       </c>
     </row>
     <row r="97" spans="1:1">

</xml_diff>

<commit_message>
First iPhone Implementation, creating abstract class for preparing iPhone integration
</commit_message>
<xml_diff>
--- a/Project Statistics/LOC.xlsx
+++ b/Project Statistics/LOC.xlsx
@@ -643,6 +643,9 @@
                 <c:pt idx="94">
                   <c:v>9925.0</c:v>
                 </c:pt>
+                <c:pt idx="98">
+                  <c:v>10147.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -656,11 +659,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2077291224"/>
-        <c:axId val="2077294168"/>
+        <c:axId val="2098709608"/>
+        <c:axId val="2098712536"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="2077291224"/>
+        <c:axId val="2098709608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -670,14 +673,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2077294168"/>
+        <c:crossAx val="2098712536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2077294168"/>
+        <c:axId val="2098712536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -688,7 +691,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2077291224"/>
+        <c:crossAx val="2098709608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1069,8 +1072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView tabSelected="1" topLeftCell="B60" workbookViewId="0">
+      <selection activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1713,67 +1716,70 @@
         <v>9925</v>
       </c>
     </row>
-    <row r="97" spans="1:1">
+    <row r="97" spans="1:2">
       <c r="A97" s="1">
         <v>41827</v>
       </c>
     </row>
-    <row r="98" spans="1:1">
+    <row r="98" spans="1:2">
       <c r="A98" s="1">
         <v>41828</v>
       </c>
     </row>
-    <row r="99" spans="1:1">
+    <row r="99" spans="1:2">
       <c r="A99" s="1">
         <v>41829</v>
       </c>
     </row>
-    <row r="100" spans="1:1">
+    <row r="100" spans="1:2">
       <c r="A100" s="1">
         <v>41830</v>
       </c>
-    </row>
-    <row r="101" spans="1:1">
+      <c r="B100">
+        <v>10147</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
       <c r="A101" s="1">
         <v>41831</v>
       </c>
     </row>
-    <row r="102" spans="1:1">
+    <row r="102" spans="1:2">
       <c r="A102" s="1">
         <v>41832</v>
       </c>
     </row>
-    <row r="103" spans="1:1">
+    <row r="103" spans="1:2">
       <c r="A103" s="1">
         <v>41833</v>
       </c>
     </row>
-    <row r="104" spans="1:1">
+    <row r="104" spans="1:2">
       <c r="A104" s="1">
         <v>41834</v>
       </c>
     </row>
-    <row r="105" spans="1:1">
+    <row r="105" spans="1:2">
       <c r="A105" s="1">
         <v>41835</v>
       </c>
     </row>
-    <row r="106" spans="1:1">
+    <row r="106" spans="1:2">
       <c r="A106" s="1">
         <v>41836</v>
       </c>
     </row>
-    <row r="107" spans="1:1">
+    <row r="107" spans="1:2">
       <c r="A107" s="1">
         <v>41837</v>
       </c>
     </row>
-    <row r="108" spans="1:1">
+    <row r="108" spans="1:2">
       <c r="A108" s="1">
         <v>41838</v>
       </c>
     </row>
-    <row r="109" spans="1:1">
+    <row r="109" spans="1:2">
       <c r="A109" s="1">
         <v>41839</v>
       </c>

</xml_diff>

<commit_message>
Added Program Home View Controller code for iPhone
</commit_message>
<xml_diff>
--- a/Project Statistics/LOC.xlsx
+++ b/Project Statistics/LOC.xlsx
@@ -189,10 +189,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$109</c:f>
+              <c:f>Sheet1!$A$2:$A$115</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="108"/>
+                <c:ptCount val="114"/>
                 <c:pt idx="0">
                   <c:v>41732.0</c:v>
                 </c:pt>
@@ -516,16 +516,34 @@
                 </c:pt>
                 <c:pt idx="107">
                   <c:v>41839.0</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>41840.0</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>41841.0</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>41842.0</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>41843.0</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>41844.0</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>41845.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$109</c:f>
+              <c:f>Sheet1!$B$2:$B$115</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="108"/>
+                <c:ptCount val="114"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
@@ -645,6 +663,12 @@
                 </c:pt>
                 <c:pt idx="98">
                   <c:v>10147.0</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>10606.0</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>11111.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -659,11 +683,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2098709608"/>
-        <c:axId val="2098712536"/>
+        <c:axId val="2093793784"/>
+        <c:axId val="2093796728"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="2098709608"/>
+        <c:axId val="2093793784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -673,14 +697,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2098712536"/>
+        <c:crossAx val="2093796728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2098712536"/>
+        <c:axId val="2093796728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -691,7 +715,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2098709608"/>
+        <c:crossAx val="2093793784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1070,10 +1094,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D109"/>
+  <dimension ref="A1:D115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B60" workbookViewId="0">
-      <selection activeCell="D96" sqref="D96"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="H73" sqref="H73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1748,11 +1772,17 @@
       <c r="A102" s="1">
         <v>41832</v>
       </c>
+      <c r="B102">
+        <v>10606</v>
+      </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" s="1">
         <v>41833</v>
       </c>
+      <c r="B103">
+        <v>11111</v>
+      </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" s="1">
@@ -1782,6 +1812,36 @@
     <row r="109" spans="1:2">
       <c r="A109" s="1">
         <v>41839</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" s="1">
+        <v>41840</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" s="1">
+        <v>41841</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" s="1">
+        <v>41842</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" s="1">
+        <v>41843</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" s="1">
+        <v>41844</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" s="1">
+        <v>41845</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Program Academics Progress View Label feature and Updated Screenshots
</commit_message>
<xml_diff>
--- a/Project Statistics/LOC.xlsx
+++ b/Project Statistics/LOC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-24180" yWindow="5600" windowWidth="24180" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24260" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -67,6 +67,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -670,6 +671,9 @@
                 <c:pt idx="101">
                   <c:v>11111.0</c:v>
                 </c:pt>
+                <c:pt idx="108">
+                  <c:v>12599.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -683,11 +687,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2093793784"/>
-        <c:axId val="2093796728"/>
+        <c:axId val="2106599864"/>
+        <c:axId val="2106596984"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="2093793784"/>
+        <c:axId val="2106599864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -697,14 +701,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2093796728"/>
+        <c:crossAx val="2106596984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2093796728"/>
+        <c:axId val="2106596984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -715,7 +719,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2093793784"/>
+        <c:crossAx val="2106599864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1096,8 +1100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="H73" sqref="H73"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1818,6 +1822,9 @@
       <c r="A110" s="1">
         <v>41840</v>
       </c>
+      <c r="B110">
+        <v>12599</v>
+      </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" s="1">

</xml_diff>